<commit_message>
dynamic reader and datatype from file added
</commit_message>
<xml_diff>
--- a/test_data/qa/test_data.xlsx
+++ b/test_data/qa/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2067A5DA-332E-4AF3-81A0-14EA518F9D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A669F7-6ECC-4DBE-BE3A-574CC9259BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>email</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>login_data</t>
+  </si>
+  <si>
+    <t>signup</t>
   </si>
 </sst>
 </file>
@@ -101,27 +107,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -144,19 +135,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -442,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45A51-54AD-4EB2-9CAD-EE9C14BB949C}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,18 +448,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -480,42 +474,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>456789</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{958ACBFA-BE59-492A-8488-406953A29FA0}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{7DA938F6-2E7F-4C79-A78F-19BF8A95B95C}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{958ACBFA-BE59-492A-8488-406953A29FA0}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{7DA938F6-2E7F-4C79-A78F-19BF8A95B95C}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{4BE6A0A7-1C86-4A69-8905-B970B1DAA1F9}"/>
+    <hyperlink ref="C9" r:id="rId4" display="5946644Ss@" xr:uid="{F3909782-B04C-4B17-87AD-59DC44295814}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
click with actions chains fixed
</commit_message>
<xml_diff>
--- a/test_data/qa/test_data.xlsx
+++ b/test_data/qa/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A669F7-6ECC-4DBE-BE3A-574CC9259BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E4EDAA-44FF-4081-8D81-153E9804ADB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="135" yWindow="1710" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>email</t>
   </si>
@@ -56,6 +56,27 @@
   </si>
   <si>
     <t>signup</t>
+  </si>
+  <si>
+    <t>headless</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>report_receiver</t>
+  </si>
+  <si>
+    <t>sompodsrkr@gmail.com</t>
+  </si>
+  <si>
+    <t>report_sender_email</t>
+  </si>
+  <si>
+    <t>report_sender_password</t>
+  </si>
+  <si>
+    <t>sompod123@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -135,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -153,6 +174,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -434,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45A51-54AD-4EB2-9CAD-EE9C14BB949C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,30 +468,60 @@
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{74098323-5AA0-4A17-BE1B-A4BE860FD756}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{4BCD1585-7AE5-4EAD-A79A-9F619E6B4349}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{B87EAD4C-FDD8-4DA4-A815-798DC67123B9}"/>
+    <hyperlink ref="F2" r:id="rId4" xr:uid="{00A0B6DE-F97D-4B81-B84B-25B626F2A816}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -476,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>

</xml_diff>